<commit_message>
Correções / Primeiras Tarefas
</commit_message>
<xml_diff>
--- a/Gabriel/Tarefas.xlsx
+++ b/Gabriel/Tarefas.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/delfos/Gabriel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\delfos\Gabriel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7418C2DA-9846-CB41-9D3A-0918D19304E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B427043A-00B6-46E7-810E-34D4DC7E518A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="57600" windowHeight="35500" xr2:uid="{07C6B7F1-DC0F-8843-8838-350D9F4D3B18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{07C6B7F1-DC0F-8843-8838-350D9F4D3B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,15 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
   <si>
     <t>Pendente</t>
   </si>
   <si>
     <t>OK</t>
-  </si>
-  <si>
-    <t>em //Consulta para Select - BEGIN adicionar: "WHERE tabela.status = 1"</t>
   </si>
   <si>
     <t>Todas páginas model/.../salvar_.....php que salvam "id" de outra tabela</t>
@@ -68,9 +63,6 @@
     <t>OBS</t>
   </si>
   <si>
-    <t>Exemplo: model/ensino_modalidade_etapa/savlar_ensino_modalidade_etapa.php</t>
-  </si>
-  <si>
     <t>Tarefa Correção</t>
   </si>
   <si>
@@ -84,9 +76,6 @@
   </si>
   <si>
     <t>Exemplo: view/ensino_modalidade_etapa/listar.php</t>
-  </si>
-  <si>
-    <t>Todas páginas view/.../visualizar.php e visualizar.php que relacionam com outra tabela</t>
   </si>
   <si>
     <t>Exemplo: view/ensino_modalidade_etapa/visualizar.php</t>
@@ -188,17 +177,23 @@
     <t>Correção</t>
   </si>
   <si>
-    <t>Gabriel Fazrer "Tarefa Correção"</t>
+    <t>Tarefa Validada e finalizada</t>
   </si>
   <si>
-    <t>Tarefa Validada e finalizada</t>
+    <t>Gabriel Fazer "Tarefa Correção"</t>
+  </si>
+  <si>
+    <t>em //Consulta para Select - BEGIN adicionar: "WHERE abv.status = 1"</t>
+  </si>
+  <si>
+    <t>Exemplo: model/ensino_modalidade_etapa/salvar_ensino_modalidade_etapa.php</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,6 +203,15 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -250,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -259,6 +263,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,183 +580,183 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DB4402F-8E19-A444-B057-57F554C57F6A}">
   <dimension ref="A2:F497"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="4"/>
-    <col min="3" max="3" width="73.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.1640625" customWidth="1"/>
+    <col min="1" max="1" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="4"/>
+    <col min="3" max="3" width="73.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.125" customWidth="1"/>
     <col min="6" max="6" width="70.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>6</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>7</v>
       </c>
@@ -759,15 +764,15 @@
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -775,15 +780,15 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -791,15 +796,15 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>10</v>
       </c>
@@ -807,15 +812,15 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>11</v>
       </c>
@@ -823,15 +828,15 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>12</v>
       </c>
@@ -839,15 +844,15 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>13</v>
       </c>
@@ -855,15 +860,15 @@
         <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>14</v>
       </c>
@@ -871,15 +876,15 @@
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>15</v>
       </c>
@@ -887,15 +892,15 @@
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>16</v>
       </c>
@@ -903,15 +908,15 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>17</v>
       </c>
@@ -919,15 +924,15 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>18</v>
       </c>
@@ -935,15 +940,15 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>19</v>
       </c>
@@ -951,15 +956,15 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>20</v>
       </c>
@@ -967,15 +972,15 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>21</v>
       </c>
@@ -983,15 +988,15 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>22</v>
       </c>
@@ -999,15 +1004,15 @@
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>23</v>
       </c>
@@ -1015,15 +1020,15 @@
         <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>24</v>
       </c>
@@ -1031,15 +1036,15 @@
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>25</v>
       </c>
@@ -1047,15 +1052,15 @@
         <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>26</v>
       </c>
@@ -1063,15 +1068,15 @@
         <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>27</v>
       </c>
@@ -1079,15 +1084,15 @@
         <v>0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>28</v>
       </c>
@@ -1095,15 +1100,15 @@
         <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>29</v>
       </c>
@@ -1113,7 +1118,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>30</v>
       </c>
@@ -1123,7 +1128,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>31</v>
       </c>
@@ -1133,7 +1138,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>32</v>
       </c>
@@ -1143,7 +1148,7 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>33</v>
       </c>
@@ -1153,7 +1158,7 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>34</v>
       </c>
@@ -1163,7 +1168,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>35</v>
       </c>
@@ -1173,7 +1178,7 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>36</v>
       </c>
@@ -1183,7 +1188,7 @@
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>37</v>
       </c>
@@ -1193,7 +1198,7 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>38</v>
       </c>
@@ -1203,7 +1208,7 @@
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>39</v>
       </c>
@@ -1213,7 +1218,7 @@
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>40</v>
       </c>
@@ -1223,7 +1228,7 @@
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>41</v>
       </c>
@@ -1233,7 +1238,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>42</v>
       </c>
@@ -1243,7 +1248,7 @@
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43</v>
       </c>
@@ -1253,7 +1258,7 @@
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44</v>
       </c>
@@ -1263,7 +1268,7 @@
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45</v>
       </c>
@@ -1273,7 +1278,7 @@
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>46</v>
       </c>
@@ -1283,7 +1288,7 @@
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>47</v>
       </c>
@@ -1293,7 +1298,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>48</v>
       </c>
@@ -1303,7 +1308,7 @@
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>49</v>
       </c>
@@ -1313,7 +1318,7 @@
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>50</v>
       </c>
@@ -1323,7 +1328,7 @@
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>51</v>
       </c>
@@ -1333,7 +1338,7 @@
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>52</v>
       </c>
@@ -1343,7 +1348,7 @@
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>53</v>
       </c>
@@ -1353,7 +1358,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>54</v>
       </c>
@@ -1363,7 +1368,7 @@
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>55</v>
       </c>
@@ -1373,7 +1378,7 @@
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>56</v>
       </c>
@@ -1383,7 +1388,7 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>57</v>
       </c>
@@ -1393,7 +1398,7 @@
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>58</v>
       </c>
@@ -1403,7 +1408,7 @@
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>59</v>
       </c>
@@ -1413,7 +1418,7 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>60</v>
       </c>
@@ -1423,7 +1428,7 @@
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>61</v>
       </c>
@@ -1433,7 +1438,7 @@
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>62</v>
       </c>
@@ -1443,7 +1448,7 @@
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>63</v>
       </c>
@@ -1453,7 +1458,7 @@
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>64</v>
       </c>
@@ -1463,7 +1468,7 @@
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>65</v>
       </c>
@@ -1473,7 +1478,7 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>66</v>
       </c>
@@ -1483,7 +1488,7 @@
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>67</v>
       </c>
@@ -1493,7 +1498,7 @@
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>68</v>
       </c>
@@ -1503,7 +1508,7 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>69</v>
       </c>
@@ -1513,7 +1518,7 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>70</v>
       </c>
@@ -1523,7 +1528,7 @@
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>71</v>
       </c>
@@ -1533,7 +1538,7 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>72</v>
       </c>
@@ -1543,7 +1548,7 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>73</v>
       </c>
@@ -1553,7 +1558,7 @@
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>74</v>
       </c>
@@ -1563,7 +1568,7 @@
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>75</v>
       </c>
@@ -1573,7 +1578,7 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>76</v>
       </c>
@@ -1583,7 +1588,7 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>77</v>
       </c>
@@ -1593,7 +1598,7 @@
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>78</v>
       </c>
@@ -1603,7 +1608,7 @@
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>79</v>
       </c>
@@ -1613,7 +1618,7 @@
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>80</v>
       </c>
@@ -1623,7 +1628,7 @@
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>81</v>
       </c>
@@ -1633,7 +1638,7 @@
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>82</v>
       </c>
@@ -1643,7 +1648,7 @@
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>83</v>
       </c>
@@ -1653,7 +1658,7 @@
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>84</v>
       </c>
@@ -1663,7 +1668,7 @@
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>85</v>
       </c>
@@ -1673,7 +1678,7 @@
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>86</v>
       </c>
@@ -1683,7 +1688,7 @@
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>87</v>
       </c>
@@ -1693,7 +1698,7 @@
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>88</v>
       </c>
@@ -1703,7 +1708,7 @@
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>89</v>
       </c>
@@ -1713,7 +1718,7 @@
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>90</v>
       </c>
@@ -1723,7 +1728,7 @@
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>91</v>
       </c>
@@ -1733,7 +1738,7 @@
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>92</v>
       </c>
@@ -1743,7 +1748,7 @@
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>93</v>
       </c>
@@ -1753,7 +1758,7 @@
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>94</v>
       </c>
@@ -1763,7 +1768,7 @@
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>95</v>
       </c>
@@ -1773,7 +1778,7 @@
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>96</v>
       </c>
@@ -1783,7 +1788,7 @@
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>97</v>
       </c>
@@ -1793,7 +1798,7 @@
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>98</v>
       </c>
@@ -1803,7 +1808,7 @@
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>99</v>
       </c>
@@ -1813,7 +1818,7 @@
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>100</v>
       </c>
@@ -1823,7 +1828,7 @@
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>101</v>
       </c>
@@ -1833,7 +1838,7 @@
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>102</v>
       </c>
@@ -1843,7 +1848,7 @@
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>103</v>
       </c>
@@ -1853,7 +1858,7 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>104</v>
       </c>
@@ -1863,7 +1868,7 @@
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>105</v>
       </c>
@@ -1873,7 +1878,7 @@
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>106</v>
       </c>
@@ -1883,7 +1888,7 @@
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>107</v>
       </c>
@@ -1893,7 +1898,7 @@
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>108</v>
       </c>
@@ -1903,7 +1908,7 @@
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>109</v>
       </c>
@@ -1913,7 +1918,7 @@
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>110</v>
       </c>
@@ -1923,7 +1928,7 @@
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>111</v>
       </c>
@@ -1933,7 +1938,7 @@
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>112</v>
       </c>
@@ -1943,7 +1948,7 @@
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>113</v>
       </c>
@@ -1953,7 +1958,7 @@
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>114</v>
       </c>
@@ -1963,7 +1968,7 @@
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>115</v>
       </c>
@@ -1973,7 +1978,7 @@
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>116</v>
       </c>
@@ -1983,7 +1988,7 @@
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>117</v>
       </c>
@@ -1993,7 +1998,7 @@
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>118</v>
       </c>
@@ -2003,7 +2008,7 @@
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>119</v>
       </c>
@@ -2013,7 +2018,7 @@
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>120</v>
       </c>
@@ -2023,7 +2028,7 @@
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>121</v>
       </c>
@@ -2033,7 +2038,7 @@
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>122</v>
       </c>
@@ -2043,7 +2048,7 @@
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>123</v>
       </c>
@@ -2053,7 +2058,7 @@
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>124</v>
       </c>
@@ -2063,7 +2068,7 @@
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>125</v>
       </c>
@@ -2073,7 +2078,7 @@
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>126</v>
       </c>
@@ -2083,7 +2088,7 @@
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>127</v>
       </c>
@@ -2093,7 +2098,7 @@
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>128</v>
       </c>
@@ -2103,7 +2108,7 @@
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>129</v>
       </c>
@@ -2113,7 +2118,7 @@
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>130</v>
       </c>
@@ -2123,7 +2128,7 @@
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>131</v>
       </c>
@@ -2133,7 +2138,7 @@
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>132</v>
       </c>
@@ -2143,7 +2148,7 @@
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>133</v>
       </c>
@@ -2153,7 +2158,7 @@
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>134</v>
       </c>
@@ -2163,7 +2168,7 @@
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>135</v>
       </c>
@@ -2173,7 +2178,7 @@
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>136</v>
       </c>
@@ -2183,7 +2188,7 @@
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>137</v>
       </c>
@@ -2193,7 +2198,7 @@
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>138</v>
       </c>
@@ -2203,7 +2208,7 @@
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>139</v>
       </c>
@@ -2213,7 +2218,7 @@
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>140</v>
       </c>
@@ -2223,7 +2228,7 @@
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>141</v>
       </c>
@@ -2233,7 +2238,7 @@
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>142</v>
       </c>
@@ -2243,7 +2248,7 @@
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>143</v>
       </c>
@@ -2253,7 +2258,7 @@
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>144</v>
       </c>
@@ -2263,7 +2268,7 @@
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>145</v>
       </c>
@@ -2273,7 +2278,7 @@
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>146</v>
       </c>
@@ -2283,7 +2288,7 @@
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>147</v>
       </c>
@@ -2293,7 +2298,7 @@
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>148</v>
       </c>
@@ -2303,7 +2308,7 @@
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>149</v>
       </c>
@@ -2313,7 +2318,7 @@
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>150</v>
       </c>
@@ -2323,7 +2328,7 @@
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>151</v>
       </c>
@@ -2333,7 +2338,7 @@
       <c r="E160" s="1"/>
       <c r="F160" s="1"/>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>152</v>
       </c>
@@ -2343,7 +2348,7 @@
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>153</v>
       </c>
@@ -2353,7 +2358,7 @@
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>154</v>
       </c>
@@ -2363,7 +2368,7 @@
       <c r="E163" s="1"/>
       <c r="F163" s="1"/>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>155</v>
       </c>
@@ -2373,7 +2378,7 @@
       <c r="E164" s="1"/>
       <c r="F164" s="1"/>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>156</v>
       </c>
@@ -2383,7 +2388,7 @@
       <c r="E165" s="1"/>
       <c r="F165" s="1"/>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>157</v>
       </c>
@@ -2393,7 +2398,7 @@
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>158</v>
       </c>
@@ -2403,7 +2408,7 @@
       <c r="E167" s="1"/>
       <c r="F167" s="1"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>159</v>
       </c>
@@ -2413,7 +2418,7 @@
       <c r="E168" s="1"/>
       <c r="F168" s="1"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>160</v>
       </c>
@@ -2423,7 +2428,7 @@
       <c r="E169" s="1"/>
       <c r="F169" s="1"/>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>161</v>
       </c>
@@ -2433,7 +2438,7 @@
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>162</v>
       </c>
@@ -2443,7 +2448,7 @@
       <c r="E171" s="1"/>
       <c r="F171" s="1"/>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>163</v>
       </c>
@@ -2453,7 +2458,7 @@
       <c r="E172" s="1"/>
       <c r="F172" s="1"/>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>164</v>
       </c>
@@ -2463,7 +2468,7 @@
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>165</v>
       </c>
@@ -2473,7 +2478,7 @@
       <c r="E174" s="1"/>
       <c r="F174" s="1"/>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>166</v>
       </c>
@@ -2483,7 +2488,7 @@
       <c r="E175" s="1"/>
       <c r="F175" s="1"/>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>167</v>
       </c>
@@ -2493,7 +2498,7 @@
       <c r="E176" s="1"/>
       <c r="F176" s="1"/>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>168</v>
       </c>
@@ -2503,7 +2508,7 @@
       <c r="E177" s="1"/>
       <c r="F177" s="1"/>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>169</v>
       </c>
@@ -2513,7 +2518,7 @@
       <c r="E178" s="1"/>
       <c r="F178" s="1"/>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>170</v>
       </c>
@@ -2523,7 +2528,7 @@
       <c r="E179" s="1"/>
       <c r="F179" s="1"/>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>171</v>
       </c>
@@ -2533,7 +2538,7 @@
       <c r="E180" s="1"/>
       <c r="F180" s="1"/>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>172</v>
       </c>
@@ -2543,7 +2548,7 @@
       <c r="E181" s="1"/>
       <c r="F181" s="1"/>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>173</v>
       </c>
@@ -2553,7 +2558,7 @@
       <c r="E182" s="1"/>
       <c r="F182" s="1"/>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>174</v>
       </c>
@@ -2563,7 +2568,7 @@
       <c r="E183" s="1"/>
       <c r="F183" s="1"/>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>175</v>
       </c>
@@ -2573,7 +2578,7 @@
       <c r="E184" s="1"/>
       <c r="F184" s="1"/>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>176</v>
       </c>
@@ -2583,7 +2588,7 @@
       <c r="E185" s="1"/>
       <c r="F185" s="1"/>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>177</v>
       </c>
@@ -2593,7 +2598,7 @@
       <c r="E186" s="1"/>
       <c r="F186" s="1"/>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>178</v>
       </c>
@@ -2603,7 +2608,7 @@
       <c r="E187" s="1"/>
       <c r="F187" s="1"/>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>179</v>
       </c>
@@ -2613,7 +2618,7 @@
       <c r="E188" s="1"/>
       <c r="F188" s="1"/>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>180</v>
       </c>
@@ -2623,7 +2628,7 @@
       <c r="E189" s="1"/>
       <c r="F189" s="1"/>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>181</v>
       </c>
@@ -2633,7 +2638,7 @@
       <c r="E190" s="1"/>
       <c r="F190" s="1"/>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>182</v>
       </c>
@@ -2643,7 +2648,7 @@
       <c r="E191" s="1"/>
       <c r="F191" s="1"/>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>183</v>
       </c>
@@ -2653,7 +2658,7 @@
       <c r="E192" s="1"/>
       <c r="F192" s="1"/>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>184</v>
       </c>
@@ -2663,7 +2668,7 @@
       <c r="E193" s="1"/>
       <c r="F193" s="1"/>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>185</v>
       </c>
@@ -2673,7 +2678,7 @@
       <c r="E194" s="1"/>
       <c r="F194" s="1"/>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>186</v>
       </c>
@@ -2683,7 +2688,7 @@
       <c r="E195" s="1"/>
       <c r="F195" s="1"/>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>187</v>
       </c>
@@ -2693,7 +2698,7 @@
       <c r="E196" s="1"/>
       <c r="F196" s="1"/>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>188</v>
       </c>
@@ -2703,7 +2708,7 @@
       <c r="E197" s="1"/>
       <c r="F197" s="1"/>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>189</v>
       </c>
@@ -2713,7 +2718,7 @@
       <c r="E198" s="1"/>
       <c r="F198" s="1"/>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>190</v>
       </c>
@@ -2723,7 +2728,7 @@
       <c r="E199" s="1"/>
       <c r="F199" s="1"/>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>191</v>
       </c>
@@ -2733,7 +2738,7 @@
       <c r="E200" s="1"/>
       <c r="F200" s="1"/>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>192</v>
       </c>
@@ -2743,7 +2748,7 @@
       <c r="E201" s="1"/>
       <c r="F201" s="1"/>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>193</v>
       </c>
@@ -2753,7 +2758,7 @@
       <c r="E202" s="1"/>
       <c r="F202" s="1"/>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>194</v>
       </c>
@@ -2763,7 +2768,7 @@
       <c r="E203" s="1"/>
       <c r="F203" s="1"/>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>195</v>
       </c>
@@ -2773,7 +2778,7 @@
       <c r="E204" s="1"/>
       <c r="F204" s="1"/>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>196</v>
       </c>
@@ -2783,7 +2788,7 @@
       <c r="E205" s="1"/>
       <c r="F205" s="1"/>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>197</v>
       </c>
@@ -2793,7 +2798,7 @@
       <c r="E206" s="1"/>
       <c r="F206" s="1"/>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>198</v>
       </c>
@@ -2803,7 +2808,7 @@
       <c r="E207" s="1"/>
       <c r="F207" s="1"/>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>199</v>
       </c>
@@ -2813,7 +2818,7 @@
       <c r="E208" s="1"/>
       <c r="F208" s="1"/>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>200</v>
       </c>
@@ -2823,7 +2828,7 @@
       <c r="E209" s="1"/>
       <c r="F209" s="1"/>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>201</v>
       </c>
@@ -2833,7 +2838,7 @@
       <c r="E210" s="1"/>
       <c r="F210" s="1"/>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>202</v>
       </c>
@@ -2843,7 +2848,7 @@
       <c r="E211" s="1"/>
       <c r="F211" s="1"/>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>203</v>
       </c>
@@ -2853,7 +2858,7 @@
       <c r="E212" s="1"/>
       <c r="F212" s="1"/>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>204</v>
       </c>
@@ -2863,7 +2868,7 @@
       <c r="E213" s="1"/>
       <c r="F213" s="1"/>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>205</v>
       </c>
@@ -2873,7 +2878,7 @@
       <c r="E214" s="1"/>
       <c r="F214" s="1"/>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>206</v>
       </c>
@@ -2883,7 +2888,7 @@
       <c r="E215" s="1"/>
       <c r="F215" s="1"/>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>207</v>
       </c>
@@ -2893,7 +2898,7 @@
       <c r="E216" s="1"/>
       <c r="F216" s="1"/>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>208</v>
       </c>
@@ -2903,7 +2908,7 @@
       <c r="E217" s="1"/>
       <c r="F217" s="1"/>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>209</v>
       </c>
@@ -2913,7 +2918,7 @@
       <c r="E218" s="1"/>
       <c r="F218" s="1"/>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>210</v>
       </c>
@@ -2923,7 +2928,7 @@
       <c r="E219" s="1"/>
       <c r="F219" s="1"/>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>211</v>
       </c>
@@ -2933,7 +2938,7 @@
       <c r="E220" s="1"/>
       <c r="F220" s="1"/>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>212</v>
       </c>
@@ -2943,7 +2948,7 @@
       <c r="E221" s="1"/>
       <c r="F221" s="1"/>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>213</v>
       </c>
@@ -2953,7 +2958,7 @@
       <c r="E222" s="1"/>
       <c r="F222" s="1"/>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>214</v>
       </c>
@@ -2963,7 +2968,7 @@
       <c r="E223" s="1"/>
       <c r="F223" s="1"/>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>215</v>
       </c>
@@ -2973,7 +2978,7 @@
       <c r="E224" s="1"/>
       <c r="F224" s="1"/>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>216</v>
       </c>
@@ -2983,7 +2988,7 @@
       <c r="E225" s="1"/>
       <c r="F225" s="1"/>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>217</v>
       </c>
@@ -2993,7 +2998,7 @@
       <c r="E226" s="1"/>
       <c r="F226" s="1"/>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>218</v>
       </c>
@@ -3003,7 +3008,7 @@
       <c r="E227" s="1"/>
       <c r="F227" s="1"/>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>219</v>
       </c>
@@ -3013,7 +3018,7 @@
       <c r="E228" s="1"/>
       <c r="F228" s="1"/>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>220</v>
       </c>
@@ -3023,7 +3028,7 @@
       <c r="E229" s="1"/>
       <c r="F229" s="1"/>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>221</v>
       </c>
@@ -3033,7 +3038,7 @@
       <c r="E230" s="1"/>
       <c r="F230" s="1"/>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>222</v>
       </c>
@@ -3043,7 +3048,7 @@
       <c r="E231" s="1"/>
       <c r="F231" s="1"/>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>223</v>
       </c>
@@ -3053,7 +3058,7 @@
       <c r="E232" s="1"/>
       <c r="F232" s="1"/>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>224</v>
       </c>
@@ -3063,7 +3068,7 @@
       <c r="E233" s="1"/>
       <c r="F233" s="1"/>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>225</v>
       </c>
@@ -3073,7 +3078,7 @@
       <c r="E234" s="1"/>
       <c r="F234" s="1"/>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>226</v>
       </c>
@@ -3083,7 +3088,7 @@
       <c r="E235" s="1"/>
       <c r="F235" s="1"/>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>227</v>
       </c>
@@ -3093,7 +3098,7 @@
       <c r="E236" s="1"/>
       <c r="F236" s="1"/>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>228</v>
       </c>
@@ -3103,7 +3108,7 @@
       <c r="E237" s="1"/>
       <c r="F237" s="1"/>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>229</v>
       </c>
@@ -3113,7 +3118,7 @@
       <c r="E238" s="1"/>
       <c r="F238" s="1"/>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>230</v>
       </c>
@@ -3123,7 +3128,7 @@
       <c r="E239" s="1"/>
       <c r="F239" s="1"/>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>231</v>
       </c>
@@ -3133,7 +3138,7 @@
       <c r="E240" s="1"/>
       <c r="F240" s="1"/>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>232</v>
       </c>
@@ -3143,7 +3148,7 @@
       <c r="E241" s="1"/>
       <c r="F241" s="1"/>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>233</v>
       </c>
@@ -3153,7 +3158,7 @@
       <c r="E242" s="1"/>
       <c r="F242" s="1"/>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>234</v>
       </c>
@@ -3163,7 +3168,7 @@
       <c r="E243" s="1"/>
       <c r="F243" s="1"/>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>235</v>
       </c>
@@ -3173,7 +3178,7 @@
       <c r="E244" s="1"/>
       <c r="F244" s="1"/>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>236</v>
       </c>
@@ -3183,7 +3188,7 @@
       <c r="E245" s="1"/>
       <c r="F245" s="1"/>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>237</v>
       </c>
@@ -3193,7 +3198,7 @@
       <c r="E246" s="1"/>
       <c r="F246" s="1"/>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>238</v>
       </c>
@@ -3203,7 +3208,7 @@
       <c r="E247" s="1"/>
       <c r="F247" s="1"/>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>239</v>
       </c>
@@ -3213,7 +3218,7 @@
       <c r="E248" s="1"/>
       <c r="F248" s="1"/>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>240</v>
       </c>
@@ -3223,7 +3228,7 @@
       <c r="E249" s="1"/>
       <c r="F249" s="1"/>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>241</v>
       </c>
@@ -3233,7 +3238,7 @@
       <c r="E250" s="1"/>
       <c r="F250" s="1"/>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>242</v>
       </c>
@@ -3243,7 +3248,7 @@
       <c r="E251" s="1"/>
       <c r="F251" s="1"/>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>243</v>
       </c>
@@ -3253,7 +3258,7 @@
       <c r="E252" s="1"/>
       <c r="F252" s="1"/>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>244</v>
       </c>
@@ -3263,7 +3268,7 @@
       <c r="E253" s="1"/>
       <c r="F253" s="1"/>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>245</v>
       </c>
@@ -3273,7 +3278,7 @@
       <c r="E254" s="1"/>
       <c r="F254" s="1"/>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>246</v>
       </c>
@@ -3283,7 +3288,7 @@
       <c r="E255" s="1"/>
       <c r="F255" s="1"/>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>247</v>
       </c>
@@ -3293,7 +3298,7 @@
       <c r="E256" s="1"/>
       <c r="F256" s="1"/>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>248</v>
       </c>
@@ -3303,7 +3308,7 @@
       <c r="E257" s="1"/>
       <c r="F257" s="1"/>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>249</v>
       </c>
@@ -3313,7 +3318,7 @@
       <c r="E258" s="1"/>
       <c r="F258" s="1"/>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>250</v>
       </c>
@@ -3323,7 +3328,7 @@
       <c r="E259" s="1"/>
       <c r="F259" s="1"/>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>251</v>
       </c>
@@ -3333,7 +3338,7 @@
       <c r="E260" s="1"/>
       <c r="F260" s="1"/>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>252</v>
       </c>
@@ -3343,7 +3348,7 @@
       <c r="E261" s="1"/>
       <c r="F261" s="1"/>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>253</v>
       </c>
@@ -3353,7 +3358,7 @@
       <c r="E262" s="1"/>
       <c r="F262" s="1"/>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>254</v>
       </c>
@@ -3363,7 +3368,7 @@
       <c r="E263" s="1"/>
       <c r="F263" s="1"/>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>255</v>
       </c>
@@ -3373,7 +3378,7 @@
       <c r="E264" s="1"/>
       <c r="F264" s="1"/>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>256</v>
       </c>
@@ -3383,7 +3388,7 @@
       <c r="E265" s="1"/>
       <c r="F265" s="1"/>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>257</v>
       </c>
@@ -3393,7 +3398,7 @@
       <c r="E266" s="1"/>
       <c r="F266" s="1"/>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>258</v>
       </c>
@@ -3403,7 +3408,7 @@
       <c r="E267" s="1"/>
       <c r="F267" s="1"/>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>259</v>
       </c>
@@ -3413,7 +3418,7 @@
       <c r="E268" s="1"/>
       <c r="F268" s="1"/>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>260</v>
       </c>
@@ -3423,7 +3428,7 @@
       <c r="E269" s="1"/>
       <c r="F269" s="1"/>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>261</v>
       </c>
@@ -3433,7 +3438,7 @@
       <c r="E270" s="1"/>
       <c r="F270" s="1"/>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>262</v>
       </c>
@@ -3443,7 +3448,7 @@
       <c r="E271" s="1"/>
       <c r="F271" s="1"/>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>263</v>
       </c>
@@ -3453,7 +3458,7 @@
       <c r="E272" s="1"/>
       <c r="F272" s="1"/>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>264</v>
       </c>
@@ -3463,7 +3468,7 @@
       <c r="E273" s="1"/>
       <c r="F273" s="1"/>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>265</v>
       </c>
@@ -3473,7 +3478,7 @@
       <c r="E274" s="1"/>
       <c r="F274" s="1"/>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>266</v>
       </c>
@@ -3483,7 +3488,7 @@
       <c r="E275" s="1"/>
       <c r="F275" s="1"/>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>267</v>
       </c>
@@ -3493,7 +3498,7 @@
       <c r="E276" s="1"/>
       <c r="F276" s="1"/>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>268</v>
       </c>
@@ -3503,7 +3508,7 @@
       <c r="E277" s="1"/>
       <c r="F277" s="1"/>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>269</v>
       </c>
@@ -3513,7 +3518,7 @@
       <c r="E278" s="1"/>
       <c r="F278" s="1"/>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>270</v>
       </c>
@@ -3523,7 +3528,7 @@
       <c r="E279" s="1"/>
       <c r="F279" s="1"/>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>271</v>
       </c>
@@ -3533,7 +3538,7 @@
       <c r="E280" s="1"/>
       <c r="F280" s="1"/>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>272</v>
       </c>
@@ -3543,7 +3548,7 @@
       <c r="E281" s="1"/>
       <c r="F281" s="1"/>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>273</v>
       </c>
@@ -3553,7 +3558,7 @@
       <c r="E282" s="1"/>
       <c r="F282" s="1"/>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>274</v>
       </c>
@@ -3563,7 +3568,7 @@
       <c r="E283" s="1"/>
       <c r="F283" s="1"/>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>275</v>
       </c>
@@ -3573,7 +3578,7 @@
       <c r="E284" s="1"/>
       <c r="F284" s="1"/>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>276</v>
       </c>
@@ -3583,7 +3588,7 @@
       <c r="E285" s="1"/>
       <c r="F285" s="1"/>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>277</v>
       </c>
@@ -3593,7 +3598,7 @@
       <c r="E286" s="1"/>
       <c r="F286" s="1"/>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>278</v>
       </c>
@@ -3603,7 +3608,7 @@
       <c r="E287" s="1"/>
       <c r="F287" s="1"/>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>279</v>
       </c>
@@ -3613,7 +3618,7 @@
       <c r="E288" s="1"/>
       <c r="F288" s="1"/>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>280</v>
       </c>
@@ -3623,7 +3628,7 @@
       <c r="E289" s="1"/>
       <c r="F289" s="1"/>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>281</v>
       </c>
@@ -3633,7 +3638,7 @@
       <c r="E290" s="1"/>
       <c r="F290" s="1"/>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>282</v>
       </c>
@@ -3643,7 +3648,7 @@
       <c r="E291" s="1"/>
       <c r="F291" s="1"/>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>283</v>
       </c>
@@ -3653,7 +3658,7 @@
       <c r="E292" s="1"/>
       <c r="F292" s="1"/>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>284</v>
       </c>
@@ -3663,7 +3668,7 @@
       <c r="E293" s="1"/>
       <c r="F293" s="1"/>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>285</v>
       </c>
@@ -3673,7 +3678,7 @@
       <c r="E294" s="1"/>
       <c r="F294" s="1"/>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>286</v>
       </c>
@@ -3683,7 +3688,7 @@
       <c r="E295" s="1"/>
       <c r="F295" s="1"/>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>287</v>
       </c>
@@ -3693,7 +3698,7 @@
       <c r="E296" s="1"/>
       <c r="F296" s="1"/>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>288</v>
       </c>
@@ -3703,7 +3708,7 @@
       <c r="E297" s="1"/>
       <c r="F297" s="1"/>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>289</v>
       </c>
@@ -3713,7 +3718,7 @@
       <c r="E298" s="1"/>
       <c r="F298" s="1"/>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>290</v>
       </c>
@@ -3723,7 +3728,7 @@
       <c r="E299" s="1"/>
       <c r="F299" s="1"/>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>291</v>
       </c>
@@ -3733,7 +3738,7 @@
       <c r="E300" s="1"/>
       <c r="F300" s="1"/>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>292</v>
       </c>
@@ -3743,7 +3748,7 @@
       <c r="E301" s="1"/>
       <c r="F301" s="1"/>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>293</v>
       </c>
@@ -3753,7 +3758,7 @@
       <c r="E302" s="1"/>
       <c r="F302" s="1"/>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>294</v>
       </c>
@@ -3763,7 +3768,7 @@
       <c r="E303" s="1"/>
       <c r="F303" s="1"/>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>295</v>
       </c>
@@ -3773,7 +3778,7 @@
       <c r="E304" s="1"/>
       <c r="F304" s="1"/>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>296</v>
       </c>
@@ -3783,7 +3788,7 @@
       <c r="E305" s="1"/>
       <c r="F305" s="1"/>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>297</v>
       </c>
@@ -3793,7 +3798,7 @@
       <c r="E306" s="1"/>
       <c r="F306" s="1"/>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>298</v>
       </c>
@@ -3803,7 +3808,7 @@
       <c r="E307" s="1"/>
       <c r="F307" s="1"/>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>299</v>
       </c>
@@ -3813,7 +3818,7 @@
       <c r="E308" s="1"/>
       <c r="F308" s="1"/>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>300</v>
       </c>
@@ -3823,7 +3828,7 @@
       <c r="E309" s="1"/>
       <c r="F309" s="1"/>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>301</v>
       </c>
@@ -3833,7 +3838,7 @@
       <c r="E310" s="1"/>
       <c r="F310" s="1"/>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>302</v>
       </c>
@@ -3843,7 +3848,7 @@
       <c r="E311" s="1"/>
       <c r="F311" s="1"/>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>303</v>
       </c>
@@ -3853,7 +3858,7 @@
       <c r="E312" s="1"/>
       <c r="F312" s="1"/>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>304</v>
       </c>
@@ -3863,7 +3868,7 @@
       <c r="E313" s="1"/>
       <c r="F313" s="1"/>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>305</v>
       </c>
@@ -3873,7 +3878,7 @@
       <c r="E314" s="1"/>
       <c r="F314" s="1"/>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>306</v>
       </c>
@@ -3883,7 +3888,7 @@
       <c r="E315" s="1"/>
       <c r="F315" s="1"/>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>307</v>
       </c>
@@ -3893,7 +3898,7 @@
       <c r="E316" s="1"/>
       <c r="F316" s="1"/>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>308</v>
       </c>
@@ -3903,7 +3908,7 @@
       <c r="E317" s="1"/>
       <c r="F317" s="1"/>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>309</v>
       </c>
@@ -3913,7 +3918,7 @@
       <c r="E318" s="1"/>
       <c r="F318" s="1"/>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>310</v>
       </c>
@@ -3923,7 +3928,7 @@
       <c r="E319" s="1"/>
       <c r="F319" s="1"/>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>311</v>
       </c>
@@ -3933,7 +3938,7 @@
       <c r="E320" s="1"/>
       <c r="F320" s="1"/>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>312</v>
       </c>
@@ -3943,7 +3948,7 @@
       <c r="E321" s="1"/>
       <c r="F321" s="1"/>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>313</v>
       </c>
@@ -3953,7 +3958,7 @@
       <c r="E322" s="1"/>
       <c r="F322" s="1"/>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>314</v>
       </c>
@@ -3963,7 +3968,7 @@
       <c r="E323" s="1"/>
       <c r="F323" s="1"/>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>315</v>
       </c>
@@ -3973,7 +3978,7 @@
       <c r="E324" s="1"/>
       <c r="F324" s="1"/>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>316</v>
       </c>
@@ -3983,7 +3988,7 @@
       <c r="E325" s="1"/>
       <c r="F325" s="1"/>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>317</v>
       </c>
@@ -3993,7 +3998,7 @@
       <c r="E326" s="1"/>
       <c r="F326" s="1"/>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>318</v>
       </c>
@@ -4003,7 +4008,7 @@
       <c r="E327" s="1"/>
       <c r="F327" s="1"/>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>319</v>
       </c>
@@ -4013,7 +4018,7 @@
       <c r="E328" s="1"/>
       <c r="F328" s="1"/>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>320</v>
       </c>
@@ -4023,7 +4028,7 @@
       <c r="E329" s="1"/>
       <c r="F329" s="1"/>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>321</v>
       </c>
@@ -4033,7 +4038,7 @@
       <c r="E330" s="1"/>
       <c r="F330" s="1"/>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>322</v>
       </c>
@@ -4043,7 +4048,7 @@
       <c r="E331" s="1"/>
       <c r="F331" s="1"/>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>323</v>
       </c>
@@ -4053,7 +4058,7 @@
       <c r="E332" s="1"/>
       <c r="F332" s="1"/>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>324</v>
       </c>
@@ -4063,7 +4068,7 @@
       <c r="E333" s="1"/>
       <c r="F333" s="1"/>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>325</v>
       </c>
@@ -4073,7 +4078,7 @@
       <c r="E334" s="1"/>
       <c r="F334" s="1"/>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>326</v>
       </c>
@@ -4083,7 +4088,7 @@
       <c r="E335" s="1"/>
       <c r="F335" s="1"/>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>327</v>
       </c>
@@ -4093,7 +4098,7 @@
       <c r="E336" s="1"/>
       <c r="F336" s="1"/>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>328</v>
       </c>
@@ -4103,7 +4108,7 @@
       <c r="E337" s="1"/>
       <c r="F337" s="1"/>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>329</v>
       </c>
@@ -4113,7 +4118,7 @@
       <c r="E338" s="1"/>
       <c r="F338" s="1"/>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>330</v>
       </c>
@@ -4123,7 +4128,7 @@
       <c r="E339" s="1"/>
       <c r="F339" s="1"/>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>331</v>
       </c>
@@ -4133,7 +4138,7 @@
       <c r="E340" s="1"/>
       <c r="F340" s="1"/>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>332</v>
       </c>
@@ -4143,7 +4148,7 @@
       <c r="E341" s="1"/>
       <c r="F341" s="1"/>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>333</v>
       </c>
@@ -4153,7 +4158,7 @@
       <c r="E342" s="1"/>
       <c r="F342" s="1"/>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>334</v>
       </c>
@@ -4163,7 +4168,7 @@
       <c r="E343" s="1"/>
       <c r="F343" s="1"/>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>335</v>
       </c>
@@ -4173,7 +4178,7 @@
       <c r="E344" s="1"/>
       <c r="F344" s="1"/>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>336</v>
       </c>
@@ -4183,7 +4188,7 @@
       <c r="E345" s="1"/>
       <c r="F345" s="1"/>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>337</v>
       </c>
@@ -4193,7 +4198,7 @@
       <c r="E346" s="1"/>
       <c r="F346" s="1"/>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>338</v>
       </c>
@@ -4203,7 +4208,7 @@
       <c r="E347" s="1"/>
       <c r="F347" s="1"/>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>339</v>
       </c>
@@ -4213,7 +4218,7 @@
       <c r="E348" s="1"/>
       <c r="F348" s="1"/>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>340</v>
       </c>
@@ -4223,7 +4228,7 @@
       <c r="E349" s="1"/>
       <c r="F349" s="1"/>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>341</v>
       </c>
@@ -4233,7 +4238,7 @@
       <c r="E350" s="1"/>
       <c r="F350" s="1"/>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>342</v>
       </c>
@@ -4243,7 +4248,7 @@
       <c r="E351" s="1"/>
       <c r="F351" s="1"/>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>343</v>
       </c>
@@ -4253,7 +4258,7 @@
       <c r="E352" s="1"/>
       <c r="F352" s="1"/>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>344</v>
       </c>
@@ -4263,7 +4268,7 @@
       <c r="E353" s="1"/>
       <c r="F353" s="1"/>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>345</v>
       </c>
@@ -4273,7 +4278,7 @@
       <c r="E354" s="1"/>
       <c r="F354" s="1"/>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>346</v>
       </c>
@@ -4283,7 +4288,7 @@
       <c r="E355" s="1"/>
       <c r="F355" s="1"/>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>347</v>
       </c>
@@ -4293,7 +4298,7 @@
       <c r="E356" s="1"/>
       <c r="F356" s="1"/>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>348</v>
       </c>
@@ -4303,7 +4308,7 @@
       <c r="E357" s="1"/>
       <c r="F357" s="1"/>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>349</v>
       </c>
@@ -4313,7 +4318,7 @@
       <c r="E358" s="1"/>
       <c r="F358" s="1"/>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>350</v>
       </c>
@@ -4323,7 +4328,7 @@
       <c r="E359" s="1"/>
       <c r="F359" s="1"/>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>351</v>
       </c>
@@ -4333,7 +4338,7 @@
       <c r="E360" s="1"/>
       <c r="F360" s="1"/>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>352</v>
       </c>
@@ -4343,7 +4348,7 @@
       <c r="E361" s="1"/>
       <c r="F361" s="1"/>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>353</v>
       </c>
@@ -4353,7 +4358,7 @@
       <c r="E362" s="1"/>
       <c r="F362" s="1"/>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>354</v>
       </c>
@@ -4363,7 +4368,7 @@
       <c r="E363" s="1"/>
       <c r="F363" s="1"/>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>355</v>
       </c>
@@ -4373,7 +4378,7 @@
       <c r="E364" s="1"/>
       <c r="F364" s="1"/>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>356</v>
       </c>
@@ -4383,7 +4388,7 @@
       <c r="E365" s="1"/>
       <c r="F365" s="1"/>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>357</v>
       </c>
@@ -4393,7 +4398,7 @@
       <c r="E366" s="1"/>
       <c r="F366" s="1"/>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>358</v>
       </c>
@@ -4403,7 +4408,7 @@
       <c r="E367" s="1"/>
       <c r="F367" s="1"/>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>359</v>
       </c>
@@ -4413,7 +4418,7 @@
       <c r="E368" s="1"/>
       <c r="F368" s="1"/>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>360</v>
       </c>
@@ -4423,7 +4428,7 @@
       <c r="E369" s="1"/>
       <c r="F369" s="1"/>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>361</v>
       </c>
@@ -4433,7 +4438,7 @@
       <c r="E370" s="1"/>
       <c r="F370" s="1"/>
     </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>362</v>
       </c>
@@ -4443,7 +4448,7 @@
       <c r="E371" s="1"/>
       <c r="F371" s="1"/>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>363</v>
       </c>
@@ -4453,7 +4458,7 @@
       <c r="E372" s="1"/>
       <c r="F372" s="1"/>
     </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>364</v>
       </c>
@@ -4463,7 +4468,7 @@
       <c r="E373" s="1"/>
       <c r="F373" s="1"/>
     </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>365</v>
       </c>
@@ -4473,7 +4478,7 @@
       <c r="E374" s="1"/>
       <c r="F374" s="1"/>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>366</v>
       </c>
@@ -4483,7 +4488,7 @@
       <c r="E375" s="1"/>
       <c r="F375" s="1"/>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <v>367</v>
       </c>
@@ -4493,7 +4498,7 @@
       <c r="E376" s="1"/>
       <c r="F376" s="1"/>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <v>368</v>
       </c>
@@ -4503,7 +4508,7 @@
       <c r="E377" s="1"/>
       <c r="F377" s="1"/>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <v>369</v>
       </c>
@@ -4513,7 +4518,7 @@
       <c r="E378" s="1"/>
       <c r="F378" s="1"/>
     </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <v>370</v>
       </c>
@@ -4523,7 +4528,7 @@
       <c r="E379" s="1"/>
       <c r="F379" s="1"/>
     </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <v>371</v>
       </c>
@@ -4533,7 +4538,7 @@
       <c r="E380" s="1"/>
       <c r="F380" s="1"/>
     </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <v>372</v>
       </c>
@@ -4543,7 +4548,7 @@
       <c r="E381" s="1"/>
       <c r="F381" s="1"/>
     </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>373</v>
       </c>
@@ -4553,7 +4558,7 @@
       <c r="E382" s="1"/>
       <c r="F382" s="1"/>
     </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
         <v>374</v>
       </c>
@@ -4563,7 +4568,7 @@
       <c r="E383" s="1"/>
       <c r="F383" s="1"/>
     </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384" s="1">
         <v>375</v>
       </c>
@@ -4573,7 +4578,7 @@
       <c r="E384" s="1"/>
       <c r="F384" s="1"/>
     </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <v>376</v>
       </c>
@@ -4583,7 +4588,7 @@
       <c r="E385" s="1"/>
       <c r="F385" s="1"/>
     </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <v>377</v>
       </c>
@@ -4593,7 +4598,7 @@
       <c r="E386" s="1"/>
       <c r="F386" s="1"/>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>378</v>
       </c>
@@ -4603,7 +4608,7 @@
       <c r="E387" s="1"/>
       <c r="F387" s="1"/>
     </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>379</v>
       </c>
@@ -4613,7 +4618,7 @@
       <c r="E388" s="1"/>
       <c r="F388" s="1"/>
     </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>380</v>
       </c>
@@ -4623,7 +4628,7 @@
       <c r="E389" s="1"/>
       <c r="F389" s="1"/>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>381</v>
       </c>
@@ -4633,7 +4638,7 @@
       <c r="E390" s="1"/>
       <c r="F390" s="1"/>
     </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>382</v>
       </c>
@@ -4643,7 +4648,7 @@
       <c r="E391" s="1"/>
       <c r="F391" s="1"/>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>383</v>
       </c>
@@ -4653,7 +4658,7 @@
       <c r="E392" s="1"/>
       <c r="F392" s="1"/>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>384</v>
       </c>
@@ -4663,7 +4668,7 @@
       <c r="E393" s="1"/>
       <c r="F393" s="1"/>
     </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>385</v>
       </c>
@@ -4673,7 +4678,7 @@
       <c r="E394" s="1"/>
       <c r="F394" s="1"/>
     </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>386</v>
       </c>
@@ -4683,7 +4688,7 @@
       <c r="E395" s="1"/>
       <c r="F395" s="1"/>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>387</v>
       </c>
@@ -4693,7 +4698,7 @@
       <c r="E396" s="1"/>
       <c r="F396" s="1"/>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>388</v>
       </c>
@@ -4703,7 +4708,7 @@
       <c r="E397" s="1"/>
       <c r="F397" s="1"/>
     </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>389</v>
       </c>
@@ -4713,7 +4718,7 @@
       <c r="E398" s="1"/>
       <c r="F398" s="1"/>
     </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>390</v>
       </c>
@@ -4723,7 +4728,7 @@
       <c r="E399" s="1"/>
       <c r="F399" s="1"/>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>391</v>
       </c>
@@ -4733,7 +4738,7 @@
       <c r="E400" s="1"/>
       <c r="F400" s="1"/>
     </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>392</v>
       </c>
@@ -4743,7 +4748,7 @@
       <c r="E401" s="1"/>
       <c r="F401" s="1"/>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>393</v>
       </c>
@@ -4753,7 +4758,7 @@
       <c r="E402" s="1"/>
       <c r="F402" s="1"/>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>394</v>
       </c>
@@ -4763,7 +4768,7 @@
       <c r="E403" s="1"/>
       <c r="F403" s="1"/>
     </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>395</v>
       </c>
@@ -4773,7 +4778,7 @@
       <c r="E404" s="1"/>
       <c r="F404" s="1"/>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>396</v>
       </c>
@@ -4783,7 +4788,7 @@
       <c r="E405" s="1"/>
       <c r="F405" s="1"/>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>397</v>
       </c>
@@ -4793,7 +4798,7 @@
       <c r="E406" s="1"/>
       <c r="F406" s="1"/>
     </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>398</v>
       </c>
@@ -4803,7 +4808,7 @@
       <c r="E407" s="1"/>
       <c r="F407" s="1"/>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>399</v>
       </c>
@@ -4813,7 +4818,7 @@
       <c r="E408" s="1"/>
       <c r="F408" s="1"/>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>400</v>
       </c>
@@ -4823,7 +4828,7 @@
       <c r="E409" s="1"/>
       <c r="F409" s="1"/>
     </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>401</v>
       </c>
@@ -4833,7 +4838,7 @@
       <c r="E410" s="1"/>
       <c r="F410" s="1"/>
     </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>402</v>
       </c>
@@ -4843,7 +4848,7 @@
       <c r="E411" s="1"/>
       <c r="F411" s="1"/>
     </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>403</v>
       </c>
@@ -4853,7 +4858,7 @@
       <c r="E412" s="1"/>
       <c r="F412" s="1"/>
     </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
         <v>404</v>
       </c>
@@ -4863,7 +4868,7 @@
       <c r="E413" s="1"/>
       <c r="F413" s="1"/>
     </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
         <v>405</v>
       </c>
@@ -4873,7 +4878,7 @@
       <c r="E414" s="1"/>
       <c r="F414" s="1"/>
     </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <v>406</v>
       </c>
@@ -4883,7 +4888,7 @@
       <c r="E415" s="1"/>
       <c r="F415" s="1"/>
     </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>407</v>
       </c>
@@ -4893,7 +4898,7 @@
       <c r="E416" s="1"/>
       <c r="F416" s="1"/>
     </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>408</v>
       </c>
@@ -4903,7 +4908,7 @@
       <c r="E417" s="1"/>
       <c r="F417" s="1"/>
     </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>409</v>
       </c>
@@ -4913,7 +4918,7 @@
       <c r="E418" s="1"/>
       <c r="F418" s="1"/>
     </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <v>410</v>
       </c>
@@ -4923,7 +4928,7 @@
       <c r="E419" s="1"/>
       <c r="F419" s="1"/>
     </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <v>411</v>
       </c>
@@ -4933,7 +4938,7 @@
       <c r="E420" s="1"/>
       <c r="F420" s="1"/>
     </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>412</v>
       </c>
@@ -4943,7 +4948,7 @@
       <c r="E421" s="1"/>
       <c r="F421" s="1"/>
     </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>413</v>
       </c>
@@ -4953,7 +4958,7 @@
       <c r="E422" s="1"/>
       <c r="F422" s="1"/>
     </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <v>414</v>
       </c>
@@ -4963,7 +4968,7 @@
       <c r="E423" s="1"/>
       <c r="F423" s="1"/>
     </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <v>415</v>
       </c>
@@ -4973,7 +4978,7 @@
       <c r="E424" s="1"/>
       <c r="F424" s="1"/>
     </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <v>416</v>
       </c>
@@ -4983,7 +4988,7 @@
       <c r="E425" s="1"/>
       <c r="F425" s="1"/>
     </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <v>417</v>
       </c>
@@ -4993,7 +4998,7 @@
       <c r="E426" s="1"/>
       <c r="F426" s="1"/>
     </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A427" s="1">
         <v>418</v>
       </c>
@@ -5003,7 +5008,7 @@
       <c r="E427" s="1"/>
       <c r="F427" s="1"/>
     </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A428" s="1">
         <v>419</v>
       </c>
@@ -5013,7 +5018,7 @@
       <c r="E428" s="1"/>
       <c r="F428" s="1"/>
     </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A429" s="1">
         <v>420</v>
       </c>
@@ -5023,7 +5028,7 @@
       <c r="E429" s="1"/>
       <c r="F429" s="1"/>
     </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A430" s="1">
         <v>421</v>
       </c>
@@ -5033,7 +5038,7 @@
       <c r="E430" s="1"/>
       <c r="F430" s="1"/>
     </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A431" s="1">
         <v>422</v>
       </c>
@@ -5043,7 +5048,7 @@
       <c r="E431" s="1"/>
       <c r="F431" s="1"/>
     </row>
-    <row r="432" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A432" s="1">
         <v>423</v>
       </c>
@@ -5053,7 +5058,7 @@
       <c r="E432" s="1"/>
       <c r="F432" s="1"/>
     </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A433" s="1">
         <v>424</v>
       </c>
@@ -5063,7 +5068,7 @@
       <c r="E433" s="1"/>
       <c r="F433" s="1"/>
     </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
         <v>425</v>
       </c>
@@ -5073,7 +5078,7 @@
       <c r="E434" s="1"/>
       <c r="F434" s="1"/>
     </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A435" s="1">
         <v>426</v>
       </c>
@@ -5083,7 +5088,7 @@
       <c r="E435" s="1"/>
       <c r="F435" s="1"/>
     </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A436" s="1">
         <v>427</v>
       </c>
@@ -5093,7 +5098,7 @@
       <c r="E436" s="1"/>
       <c r="F436" s="1"/>
     </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
         <v>428</v>
       </c>
@@ -5103,7 +5108,7 @@
       <c r="E437" s="1"/>
       <c r="F437" s="1"/>
     </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
         <v>429</v>
       </c>
@@ -5113,7 +5118,7 @@
       <c r="E438" s="1"/>
       <c r="F438" s="1"/>
     </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <v>430</v>
       </c>
@@ -5123,7 +5128,7 @@
       <c r="E439" s="1"/>
       <c r="F439" s="1"/>
     </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A440" s="1">
         <v>431</v>
       </c>
@@ -5133,7 +5138,7 @@
       <c r="E440" s="1"/>
       <c r="F440" s="1"/>
     </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <v>432</v>
       </c>
@@ -5143,7 +5148,7 @@
       <c r="E441" s="1"/>
       <c r="F441" s="1"/>
     </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>433</v>
       </c>
@@ -5153,7 +5158,7 @@
       <c r="E442" s="1"/>
       <c r="F442" s="1"/>
     </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A443" s="1">
         <v>434</v>
       </c>
@@ -5163,7 +5168,7 @@
       <c r="E443" s="1"/>
       <c r="F443" s="1"/>
     </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A444" s="1">
         <v>435</v>
       </c>
@@ -5173,7 +5178,7 @@
       <c r="E444" s="1"/>
       <c r="F444" s="1"/>
     </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A445" s="1">
         <v>436</v>
       </c>
@@ -5183,7 +5188,7 @@
       <c r="E445" s="1"/>
       <c r="F445" s="1"/>
     </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
         <v>437</v>
       </c>
@@ -5193,7 +5198,7 @@
       <c r="E446" s="1"/>
       <c r="F446" s="1"/>
     </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A447" s="1">
         <v>438</v>
       </c>
@@ -5203,7 +5208,7 @@
       <c r="E447" s="1"/>
       <c r="F447" s="1"/>
     </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A448" s="1">
         <v>439</v>
       </c>
@@ -5213,7 +5218,7 @@
       <c r="E448" s="1"/>
       <c r="F448" s="1"/>
     </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A449" s="1">
         <v>440</v>
       </c>
@@ -5223,7 +5228,7 @@
       <c r="E449" s="1"/>
       <c r="F449" s="1"/>
     </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
         <v>441</v>
       </c>
@@ -5233,7 +5238,7 @@
       <c r="E450" s="1"/>
       <c r="F450" s="1"/>
     </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A451" s="1">
         <v>442</v>
       </c>
@@ -5243,7 +5248,7 @@
       <c r="E451" s="1"/>
       <c r="F451" s="1"/>
     </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A452" s="1">
         <v>443</v>
       </c>
@@ -5253,7 +5258,7 @@
       <c r="E452" s="1"/>
       <c r="F452" s="1"/>
     </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A453" s="1">
         <v>444</v>
       </c>
@@ -5263,7 +5268,7 @@
       <c r="E453" s="1"/>
       <c r="F453" s="1"/>
     </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A454" s="1">
         <v>445</v>
       </c>
@@ -5273,7 +5278,7 @@
       <c r="E454" s="1"/>
       <c r="F454" s="1"/>
     </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A455" s="1">
         <v>446</v>
       </c>
@@ -5283,7 +5288,7 @@
       <c r="E455" s="1"/>
       <c r="F455" s="1"/>
     </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A456" s="1">
         <v>447</v>
       </c>
@@ -5293,7 +5298,7 @@
       <c r="E456" s="1"/>
       <c r="F456" s="1"/>
     </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A457" s="1">
         <v>448</v>
       </c>
@@ -5303,7 +5308,7 @@
       <c r="E457" s="1"/>
       <c r="F457" s="1"/>
     </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A458" s="1">
         <v>449</v>
       </c>
@@ -5313,7 +5318,7 @@
       <c r="E458" s="1"/>
       <c r="F458" s="1"/>
     </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A459" s="1">
         <v>450</v>
       </c>
@@ -5323,7 +5328,7 @@
       <c r="E459" s="1"/>
       <c r="F459" s="1"/>
     </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A460" s="1">
         <v>451</v>
       </c>
@@ -5333,7 +5338,7 @@
       <c r="E460" s="1"/>
       <c r="F460" s="1"/>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A461" s="1">
         <v>452</v>
       </c>
@@ -5343,7 +5348,7 @@
       <c r="E461" s="1"/>
       <c r="F461" s="1"/>
     </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A462" s="1">
         <v>453</v>
       </c>
@@ -5353,7 +5358,7 @@
       <c r="E462" s="1"/>
       <c r="F462" s="1"/>
     </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A463" s="1">
         <v>454</v>
       </c>
@@ -5363,7 +5368,7 @@
       <c r="E463" s="1"/>
       <c r="F463" s="1"/>
     </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A464" s="1">
         <v>455</v>
       </c>
@@ -5373,7 +5378,7 @@
       <c r="E464" s="1"/>
       <c r="F464" s="1"/>
     </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A465" s="1">
         <v>456</v>
       </c>
@@ -5383,7 +5388,7 @@
       <c r="E465" s="1"/>
       <c r="F465" s="1"/>
     </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A466" s="1">
         <v>457</v>
       </c>
@@ -5393,7 +5398,7 @@
       <c r="E466" s="1"/>
       <c r="F466" s="1"/>
     </row>
-    <row r="467" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A467" s="1">
         <v>458</v>
       </c>
@@ -5403,7 +5408,7 @@
       <c r="E467" s="1"/>
       <c r="F467" s="1"/>
     </row>
-    <row r="468" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A468" s="1">
         <v>459</v>
       </c>
@@ -5413,7 +5418,7 @@
       <c r="E468" s="1"/>
       <c r="F468" s="1"/>
     </row>
-    <row r="469" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A469" s="1">
         <v>460</v>
       </c>
@@ -5423,7 +5428,7 @@
       <c r="E469" s="1"/>
       <c r="F469" s="1"/>
     </row>
-    <row r="470" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A470" s="1">
         <v>461</v>
       </c>
@@ -5433,7 +5438,7 @@
       <c r="E470" s="1"/>
       <c r="F470" s="1"/>
     </row>
-    <row r="471" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A471" s="1">
         <v>462</v>
       </c>
@@ -5443,7 +5448,7 @@
       <c r="E471" s="1"/>
       <c r="F471" s="1"/>
     </row>
-    <row r="472" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A472" s="1">
         <v>463</v>
       </c>
@@ -5453,7 +5458,7 @@
       <c r="E472" s="1"/>
       <c r="F472" s="1"/>
     </row>
-    <row r="473" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A473" s="1">
         <v>464</v>
       </c>
@@ -5463,7 +5468,7 @@
       <c r="E473" s="1"/>
       <c r="F473" s="1"/>
     </row>
-    <row r="474" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A474" s="1">
         <v>465</v>
       </c>
@@ -5473,7 +5478,7 @@
       <c r="E474" s="1"/>
       <c r="F474" s="1"/>
     </row>
-    <row r="475" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A475" s="1">
         <v>466</v>
       </c>
@@ -5483,7 +5488,7 @@
       <c r="E475" s="1"/>
       <c r="F475" s="1"/>
     </row>
-    <row r="476" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A476" s="1">
         <v>467</v>
       </c>
@@ -5493,7 +5498,7 @@
       <c r="E476" s="1"/>
       <c r="F476" s="1"/>
     </row>
-    <row r="477" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A477" s="1">
         <v>468</v>
       </c>
@@ -5503,7 +5508,7 @@
       <c r="E477" s="1"/>
       <c r="F477" s="1"/>
     </row>
-    <row r="478" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A478" s="1">
         <v>469</v>
       </c>
@@ -5513,7 +5518,7 @@
       <c r="E478" s="1"/>
       <c r="F478" s="1"/>
     </row>
-    <row r="479" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A479" s="1">
         <v>470</v>
       </c>
@@ -5523,7 +5528,7 @@
       <c r="E479" s="1"/>
       <c r="F479" s="1"/>
     </row>
-    <row r="480" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A480" s="1">
         <v>471</v>
       </c>
@@ -5533,7 +5538,7 @@
       <c r="E480" s="1"/>
       <c r="F480" s="1"/>
     </row>
-    <row r="481" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A481" s="1">
         <v>472</v>
       </c>
@@ -5543,7 +5548,7 @@
       <c r="E481" s="1"/>
       <c r="F481" s="1"/>
     </row>
-    <row r="482" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A482" s="1">
         <v>473</v>
       </c>
@@ -5553,7 +5558,7 @@
       <c r="E482" s="1"/>
       <c r="F482" s="1"/>
     </row>
-    <row r="483" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A483" s="1">
         <v>474</v>
       </c>
@@ -5563,7 +5568,7 @@
       <c r="E483" s="1"/>
       <c r="F483" s="1"/>
     </row>
-    <row r="484" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A484" s="1">
         <v>475</v>
       </c>
@@ -5573,7 +5578,7 @@
       <c r="E484" s="1"/>
       <c r="F484" s="1"/>
     </row>
-    <row r="485" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A485" s="1">
         <v>476</v>
       </c>
@@ -5583,7 +5588,7 @@
       <c r="E485" s="1"/>
       <c r="F485" s="1"/>
     </row>
-    <row r="486" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A486" s="1">
         <v>477</v>
       </c>
@@ -5593,7 +5598,7 @@
       <c r="E486" s="1"/>
       <c r="F486" s="1"/>
     </row>
-    <row r="487" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A487" s="1">
         <v>478</v>
       </c>
@@ -5603,7 +5608,7 @@
       <c r="E487" s="1"/>
       <c r="F487" s="1"/>
     </row>
-    <row r="488" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A488" s="1">
         <v>479</v>
       </c>
@@ -5613,7 +5618,7 @@
       <c r="E488" s="1"/>
       <c r="F488" s="1"/>
     </row>
-    <row r="489" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A489" s="1">
         <v>480</v>
       </c>
@@ -5623,7 +5628,7 @@
       <c r="E489" s="1"/>
       <c r="F489" s="1"/>
     </row>
-    <row r="490" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A490" s="1">
         <v>481</v>
       </c>
@@ -5633,7 +5638,7 @@
       <c r="E490" s="1"/>
       <c r="F490" s="1"/>
     </row>
-    <row r="491" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A491" s="1">
         <v>482</v>
       </c>
@@ -5643,7 +5648,7 @@
       <c r="E491" s="1"/>
       <c r="F491" s="1"/>
     </row>
-    <row r="492" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A492" s="1">
         <v>483</v>
       </c>
@@ -5653,7 +5658,7 @@
       <c r="E492" s="1"/>
       <c r="F492" s="1"/>
     </row>
-    <row r="493" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A493" s="1">
         <v>484</v>
       </c>
@@ -5663,7 +5668,7 @@
       <c r="E493" s="1"/>
       <c r="F493" s="1"/>
     </row>
-    <row r="494" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A494" s="1">
         <v>485</v>
       </c>
@@ -5673,7 +5678,7 @@
       <c r="E494" s="1"/>
       <c r="F494" s="1"/>
     </row>
-    <row r="495" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A495" s="1">
         <v>486</v>
       </c>
@@ -5683,7 +5688,7 @@
       <c r="E495" s="1"/>
       <c r="F495" s="1"/>
     </row>
-    <row r="496" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A496" s="1">
         <v>487</v>
       </c>
@@ -5693,7 +5698,7 @@
       <c r="E496" s="1"/>
       <c r="F496" s="1"/>
     </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A497" s="1">
         <v>488</v>
       </c>
@@ -5708,6 +5713,6 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificação de visualizar e editar js
</commit_message>
<xml_diff>
--- a/Gabriel/Tarefas.xlsx
+++ b/Gabriel/Tarefas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="76">
   <si>
     <t>Legenda</t>
   </si>
@@ -207,13 +207,43 @@
     <t>pastas</t>
   </si>
   <si>
-    <t>criar arquivos content_identificacao.php</t>
+    <t>criar view/.../.../content_identificacao.php (duplicar cadastrar.php) ||||| model/.../.../salvar_identificacao.php (renomear)</t>
   </si>
   <si>
     <t>view/.../.../content_identificacao.php</t>
   </si>
   <si>
+    <t>Substituir includes por código $id...</t>
+  </si>
+  <si>
     <t>Alterar $rsRegistro para $rsRegistro*TabelaNome*</t>
+  </si>
+  <si>
+    <t>Remover desde o elemento &lt;main&gt; até o &lt;form&gt; e desde &lt;/form&gt; até final</t>
+  </si>
+  <si>
+    <t>Adicionar código *exibesituacao, *exibebutoes *fechamento tagPHP final</t>
+  </si>
+  <si>
+    <t>Substituir linha $id = ....</t>
+  </si>
+  <si>
+    <t>Reduzir SELECT id FROM... e somente $rsRegistro['id'] = 0;</t>
+  </si>
+  <si>
+    <t>Manter somente título e descrição da página e adicionar variáveis (exibeSituação e Butões)</t>
+  </si>
+  <si>
+    <t>adicionar atributo urltosend="bsc/.../salvar_identificacao" ao elemento &lt;form</t>
+  </si>
+  <si>
+    <t>Substituir conteudo do &lt;form&gt; por include_once...</t>
+  </si>
+  <si>
+    <t>control/.../.../cadastrar.js</t>
+  </si>
+  <si>
+    <t>Alterar params: formId, urlCurrent, urlToSend</t>
   </si>
 </sst>
 </file>
@@ -591,7 +621,7 @@
     <col customWidth="1" min="1" max="1" width="4.11"/>
     <col customWidth="1" min="2" max="3" width="10.78"/>
     <col customWidth="1" min="4" max="4" width="73.67"/>
-    <col customWidth="1" min="5" max="5" width="74.11"/>
+    <col customWidth="1" min="5" max="5" width="95.11"/>
     <col customWidth="1" min="6" max="6" width="62.11"/>
     <col customWidth="1" min="7" max="7" width="70.44"/>
     <col customWidth="1" min="8" max="27" width="11.0"/>
@@ -2269,16 +2299,12 @@
       <c r="A45" s="6">
         <v>36.0</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E45" s="6"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12" t="s">
+        <v>66</v>
+      </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="1"/>
@@ -2309,7 +2335,9 @@
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+      <c r="E46" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="1"/>
@@ -2340,7 +2368,9 @@
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+      <c r="E47" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="1"/>
@@ -2368,10 +2398,18 @@
       <c r="A48" s="6">
         <v>39.0</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="B48" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="1"/>
@@ -2402,7 +2440,9 @@
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
+      <c r="E49" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="1"/>
@@ -2433,7 +2473,9 @@
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
       <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+      <c r="E50" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="1"/>
@@ -2464,7 +2506,9 @@
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
+      <c r="E51" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
       <c r="H51" s="1"/>
@@ -2495,7 +2539,9 @@
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
       <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
+      <c r="E52" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="1"/>
@@ -2523,10 +2569,18 @@
       <c r="A53" s="6">
         <v>44.0</v>
       </c>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
+      <c r="B53" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>75</v>
+      </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="1"/>

</xml_diff>